<commit_message>
Attempting to add MultiIndex support
</commit_message>
<xml_diff>
--- a/NoOffsetCase.xlsx
+++ b/NoOffsetCase.xlsx
@@ -14,12 +14,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>two</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+  <si>
+    <t>Meal</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Thur</t>
+  </si>
+  <si>
+    <t>Tues</t>
+  </si>
+  <si>
+    <t>Weds</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Midnight Snack</t>
+  </si>
+  <si>
+    <t>Toast</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>Curry</t>
+  </si>
+  <si>
+    <t>Shmores</t>
+  </si>
+  <si>
+    <t>Hotpot</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Something Different!</t>
+  </si>
+  <si>
+    <t>Biscuits</t>
   </si>
 </sst>
 </file>
@@ -377,139 +422,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>15</v>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>17</v>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>25</v>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>